<commit_message>
Udkast til statusrapport. WBS skal ajourføres (bl.a. røde markeringer fjernes) Der bør nok knyttes en kommentar til estimering af progress - svært pga. kompleksiteten pt. med samling
</commit_message>
<xml_diff>
--- a/reports/r7/opfolgning.xlsx
+++ b/reports/r7/opfolgning.xlsx
@@ -4,24 +4,25 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="9270" windowHeight="4665" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="9270" windowHeight="4665"/>
   </bookViews>
   <sheets>
     <sheet name="Opfølgning" sheetId="1" r:id="rId1"/>
     <sheet name="Tidsregnskab" sheetId="2" r:id="rId2"/>
     <sheet name="kvalitet" sheetId="6" r:id="rId3"/>
     <sheet name="Ressourcer" sheetId="3" r:id="rId4"/>
-    <sheet name="Sheet1 (2)" sheetId="8" r:id="rId5"/>
-    <sheet name="Sheet1" sheetId="7" r:id="rId6"/>
-    <sheet name="status" sheetId="4" r:id="rId7"/>
+    <sheet name="status 13-6" sheetId="9" r:id="rId5"/>
+    <sheet name="status 05-6" sheetId="8" r:id="rId6"/>
+    <sheet name="status 30-5" sheetId="7" r:id="rId7"/>
     <sheet name="status 30-3" sheetId="5" r:id="rId8"/>
+    <sheet name="status" sheetId="4" r:id="rId9"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="102">
   <si>
     <t>Forbrugt kal. til dato</t>
   </si>
@@ -245,9 +246,6 @@
     <t>Generalprøve</t>
   </si>
   <si>
-    <t>Slutmål fastsat</t>
-  </si>
-  <si>
     <t>Budget: 900 timer i alt. 32,5 timer pr. Semesteruge, 32,5 timer pr. Dag i 3-ugers perioden. Forelæsningsaktiviteter o. Lign. Ikke medregnet.</t>
   </si>
   <si>
@@ -320,29 +318,29 @@
     <t>SGR3</t>
   </si>
   <si>
-    <t>Status 3</t>
-  </si>
-  <si>
     <t>pre-3u</t>
+  </si>
+  <si>
+    <t>Slutmål fastsat / status 3</t>
+  </si>
+  <si>
+    <t>2-robot full cycle</t>
+  </si>
+  <si>
+    <t>Status 4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="11">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <i/>
@@ -490,42 +488,41 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="16" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="16" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -534,16 +531,17 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -838,21 +836,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N23"/>
+  <dimension ref="A1:O23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="32.140625" customWidth="1"/>
     <col min="2" max="9" width="12.7109375" customWidth="1"/>
-    <col min="10" max="13" width="9.7109375" customWidth="1"/>
-    <col min="14" max="14" width="12.28515625" customWidth="1"/>
+    <col min="10" max="14" width="9.7109375" customWidth="1"/>
+    <col min="15" max="15" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="4" customFormat="1" ht="15.75" thickBot="1">
+    <row r="1" spans="1:15" s="4" customFormat="1" ht="15.75" thickBot="1">
       <c r="A1" s="4" t="s">
         <v>18</v>
       </c>
@@ -884,20 +882,23 @@
         <v>40700</v>
       </c>
       <c r="K1" s="7">
-        <v>40704</v>
-      </c>
-      <c r="L1" s="24">
+        <v>40708</v>
+      </c>
+      <c r="L1" s="7">
+        <v>40709</v>
+      </c>
+      <c r="M1" s="7">
         <v>40711</v>
       </c>
-      <c r="M1" s="24">
-        <v>40715</v>
-      </c>
       <c r="N1" s="7">
+        <v>40714</v>
+      </c>
+      <c r="O1" s="7">
         <v>40718</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="15.75" thickTop="1">
-      <c r="A2" s="26" t="s">
+    <row r="2" spans="1:15" ht="15.75" thickTop="1">
+      <c r="A2" s="25" t="s">
         <v>19</v>
       </c>
       <c r="B2">
@@ -936,11 +937,14 @@
       <c r="M2">
         <v>11</v>
       </c>
-      <c r="N2" s="2">
+      <c r="N2">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:14">
+      <c r="O2" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
@@ -953,9 +957,10 @@
       <c r="K3" s="10"/>
       <c r="L3" s="10"/>
       <c r="M3" s="10"/>
-      <c r="N3" s="5"/>
-    </row>
-    <row r="4" spans="1:14" ht="30.75" customHeight="1">
+      <c r="N3" s="10"/>
+      <c r="O3" s="5"/>
+    </row>
+    <row r="4" spans="1:15" ht="30.75" customHeight="1">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -983,87 +988,95 @@
       <c r="I4" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="J4" s="33" t="s">
+      <c r="J4" s="32" t="s">
         <v>99</v>
       </c>
-      <c r="K4" s="33" t="s">
-        <v>74</v>
-      </c>
-      <c r="L4" s="25" t="s">
+      <c r="K4" s="32" t="s">
+        <v>101</v>
+      </c>
+      <c r="L4" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="M4" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="M4" s="25" t="s">
+      <c r="N4" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="N4" s="23" t="s">
+      <c r="O4" s="23" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
-      <c r="J5" s="36" t="s">
+    <row r="5" spans="1:15">
+      <c r="J5" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="K5" s="36"/>
-      <c r="L5" s="36"/>
-      <c r="M5" s="36"/>
-    </row>
-    <row r="6" spans="1:14">
+      <c r="K5" s="35"/>
+      <c r="L5" s="35"/>
+      <c r="M5" s="35"/>
+      <c r="N5" s="35"/>
+    </row>
+    <row r="6" spans="1:15">
       <c r="A6" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="17">
-        <f>$N1-B1</f>
+        <f>$O1-B1</f>
         <v>142</v>
       </c>
       <c r="C6" s="18">
-        <f>$N1-C1</f>
+        <f>$O1-C1</f>
         <v>121</v>
       </c>
       <c r="D6" s="18">
-        <f>$N1-D1</f>
+        <f>$O1-D1</f>
         <v>93</v>
       </c>
       <c r="E6" s="18">
-        <f>$N1-E1</f>
+        <f>$O1-E1</f>
         <v>86</v>
       </c>
       <c r="F6" s="18">
-        <f>$N1-F1</f>
+        <f>$O1-F1</f>
         <v>65</v>
       </c>
       <c r="G6" s="18">
         <v>60</v>
       </c>
       <c r="H6" s="18">
-        <f>$N1-H1</f>
+        <f t="shared" ref="H6:O6" si="0">$O1-H1</f>
         <v>36</v>
       </c>
       <c r="I6" s="18">
-        <f>$N1-I1</f>
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="J6" s="11">
-        <f>$N1-J1</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="K6" s="11">
-        <f>$N1-K1</f>
-        <v>14</v>
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
       <c r="L6" s="11">
-        <f>$N1-L1</f>
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="M6" s="11">
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="M6" s="20">
-        <f>$N1-M1</f>
-        <v>3</v>
-      </c>
-      <c r="N6" s="18">
-        <f>$N1-N1</f>
+      <c r="N6" s="20">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="O6" s="18">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:15">
       <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
@@ -1090,35 +1103,39 @@
         <v>82</v>
       </c>
       <c r="H7" s="19">
-        <f t="shared" ref="H7:N7" si="0">$B6-H6</f>
+        <f t="shared" ref="H7:O7" si="1">$B6-H6</f>
         <v>106</v>
       </c>
       <c r="I7" s="19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>117</v>
       </c>
       <c r="J7" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>124</v>
       </c>
       <c r="K7" s="12">
-        <f t="shared" si="0"/>
-        <v>128</v>
+        <f t="shared" si="1"/>
+        <v>132</v>
       </c>
       <c r="L7" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
+        <v>133</v>
+      </c>
+      <c r="M7" s="12">
+        <f t="shared" si="1"/>
         <v>135</v>
       </c>
-      <c r="M7" s="21">
-        <f t="shared" si="0"/>
-        <v>139</v>
-      </c>
-      <c r="N7" s="19">
-        <f t="shared" si="0"/>
+      <c r="N7" s="21">
+        <f t="shared" si="1"/>
+        <v>138</v>
+      </c>
+      <c r="O7" s="19">
+        <f t="shared" si="1"/>
         <v>142</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:15">
       <c r="A8" s="1"/>
       <c r="B8" s="17"/>
       <c r="C8" s="18"/>
@@ -1131,10 +1148,11 @@
       <c r="J8" s="11"/>
       <c r="K8" s="11"/>
       <c r="L8" s="11"/>
-      <c r="M8" s="20"/>
-      <c r="N8" s="18"/>
-    </row>
-    <row r="9" spans="1:14">
+      <c r="M8" s="11"/>
+      <c r="N8" s="20"/>
+      <c r="O8" s="18"/>
+    </row>
+    <row r="9" spans="1:15">
       <c r="A9" s="1"/>
       <c r="B9" s="17"/>
       <c r="C9" s="18"/>
@@ -1147,10 +1165,11 @@
       <c r="J9" s="11"/>
       <c r="K9" s="11"/>
       <c r="L9" s="11"/>
-      <c r="M9" s="20"/>
-      <c r="N9" s="18"/>
-    </row>
-    <row r="10" spans="1:14">
+      <c r="M9" s="11"/>
+      <c r="N9" s="20"/>
+      <c r="O9" s="18"/>
+    </row>
+    <row r="10" spans="1:15">
       <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
@@ -1182,19 +1201,22 @@
         <v>63</v>
       </c>
       <c r="K10" s="11">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="L10" s="11">
+        <v>77</v>
+      </c>
+      <c r="M10" s="11">
         <v>80</v>
       </c>
-      <c r="M10" s="11">
+      <c r="N10" s="11">
         <v>90</v>
       </c>
-      <c r="N10" s="18">
+      <c r="O10" s="18">
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:15">
       <c r="A11" s="1" t="s">
         <v>6</v>
       </c>
@@ -1225,12 +1247,16 @@
       <c r="J11" s="11">
         <v>66</v>
       </c>
-      <c r="K11" s="11"/>
+      <c r="K11" s="36">
+        <f>'status 13-6'!$A$1*100</f>
+        <v>74.993055555555571</v>
+      </c>
       <c r="L11" s="11"/>
-      <c r="M11" s="20"/>
-      <c r="N11" s="18"/>
-    </row>
-    <row r="12" spans="1:14">
+      <c r="M11" s="11"/>
+      <c r="N11" s="20"/>
+      <c r="O11" s="18"/>
+    </row>
+    <row r="12" spans="1:15">
       <c r="B12" s="17"/>
       <c r="C12" s="18"/>
       <c r="D12" s="18"/>
@@ -1242,10 +1268,11 @@
       <c r="J12" s="11"/>
       <c r="K12" s="11"/>
       <c r="L12" s="11"/>
-      <c r="M12" s="20"/>
-      <c r="N12" s="18"/>
-    </row>
-    <row r="13" spans="1:14">
+      <c r="M12" s="11"/>
+      <c r="N12" s="20"/>
+      <c r="O12" s="18"/>
+    </row>
+    <row r="13" spans="1:15">
       <c r="A13" s="1" t="s">
         <v>7</v>
       </c>
@@ -1253,19 +1280,19 @@
         <v>0</v>
       </c>
       <c r="C13" s="18">
-        <f t="shared" ref="C13:F13" si="1">ROUND(($C$16-C16+75)/$C$16,2)*100</f>
+        <f t="shared" ref="C13:F13" si="2">ROUND(($C$16-C16+75)/$C$16,2)*100</f>
         <v>9</v>
       </c>
       <c r="D13" s="18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>26</v>
       </c>
       <c r="E13" s="18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>30</v>
       </c>
       <c r="F13" s="18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>42</v>
       </c>
       <c r="G13" s="18">
@@ -1273,11 +1300,11 @@
         <v>42</v>
       </c>
       <c r="H13" s="18">
-        <f t="shared" ref="H13:I13" si="2">ROUND(($C$16-H16+75)/$C$16,2)*100</f>
+        <f t="shared" ref="H13:I13" si="3">ROUND(($C$16-H16+75)/$C$16,2)*100</f>
         <v>50</v>
       </c>
       <c r="I13" s="18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>50</v>
       </c>
       <c r="J13" s="11">
@@ -1286,22 +1313,26 @@
       </c>
       <c r="K13" s="11">
         <f>ROUND(($C$16-K16+75)/$C$16,2)*100</f>
+        <v>66</v>
+      </c>
+      <c r="L13" s="11">
+        <f>ROUND(($C$16-L16+75)/$C$16,2)*100</f>
         <v>70</v>
       </c>
-      <c r="L13" s="11">
-        <f t="shared" ref="L13:M13" si="3">ROUND(($C$16-L16+75)/$C$16,2)*100</f>
+      <c r="M13" s="11">
+        <f t="shared" ref="M13:N13" si="4">ROUND(($C$16-M16+75)/$C$16,2)*100</f>
         <v>90</v>
       </c>
-      <c r="M13" s="11">
-        <f t="shared" si="3"/>
+      <c r="N13" s="11">
+        <f t="shared" si="4"/>
         <v>99</v>
       </c>
-      <c r="N13" s="18">
-        <f t="shared" ref="N13" si="4">ROUND(($E$16-N16)/$E$16,2)*100</f>
+      <c r="O13" s="18">
+        <f t="shared" ref="O13" si="5">ROUND(($E$16-O16)/$E$16,2)*100</f>
         <v>100</v>
       </c>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:15">
       <c r="A14" s="1" t="s">
         <v>8</v>
       </c>
@@ -1324,12 +1355,16 @@
       <c r="J14" s="11">
         <v>57</v>
       </c>
-      <c r="K14" s="11"/>
+      <c r="K14" s="36">
+        <f>kvalitet!$E$2*100</f>
+        <v>66.875</v>
+      </c>
       <c r="L14" s="11"/>
-      <c r="M14" s="20"/>
-      <c r="N14" s="18"/>
-    </row>
-    <row r="15" spans="1:14">
+      <c r="M14" s="11"/>
+      <c r="N14" s="20"/>
+      <c r="O14" s="18"/>
+    </row>
+    <row r="15" spans="1:15">
       <c r="B15" s="17"/>
       <c r="C15" s="18"/>
       <c r="D15" s="18"/>
@@ -1341,10 +1376,11 @@
       <c r="J15" s="11"/>
       <c r="K15" s="11"/>
       <c r="L15" s="11"/>
-      <c r="M15" s="20"/>
-      <c r="N15" s="18"/>
-    </row>
-    <row r="16" spans="1:14">
+      <c r="M15" s="11"/>
+      <c r="N15" s="20"/>
+      <c r="O15" s="18"/>
+    </row>
+    <row r="16" spans="1:15">
       <c r="A16" s="1" t="s">
         <v>2</v>
       </c>
@@ -1359,15 +1395,15 @@
         <f>B16-228</f>
         <v>672</v>
       </c>
-      <c r="E16" s="29">
+      <c r="E16" s="28">
         <f>B16-260</f>
         <v>640</v>
       </c>
-      <c r="F16" s="29">
+      <c r="F16" s="28">
         <f>B16-358</f>
         <v>542</v>
       </c>
-      <c r="G16" s="29">
+      <c r="G16" s="28">
         <f>B16-358</f>
         <v>542</v>
       </c>
@@ -1384,22 +1420,26 @@
         <v>445</v>
       </c>
       <c r="K16" s="11">
+        <f>B16-585+32</f>
+        <v>347</v>
+      </c>
+      <c r="L16" s="11">
         <f>B16-585</f>
         <v>315</v>
       </c>
-      <c r="L16" s="11">
+      <c r="M16" s="11">
         <f>B16-748</f>
         <v>152</v>
       </c>
-      <c r="M16" s="20">
+      <c r="N16" s="20">
         <f>B16-813</f>
         <v>87</v>
       </c>
-      <c r="N16" s="18">
+      <c r="O16" s="18">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:14">
+    <row r="17" spans="1:15">
       <c r="A17" s="1" t="s">
         <v>3</v>
       </c>
@@ -1415,35 +1455,39 @@
         <v>596.70000000000005</v>
       </c>
       <c r="E17" s="18">
-        <f t="shared" ref="E17:J17" si="5">$B$17*(100-E11)/100</f>
+        <f t="shared" ref="E17:I17" si="6">$B$17*(100-E11)/100</f>
         <v>520.20000000000005</v>
       </c>
       <c r="F17" s="18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>359.55</v>
       </c>
       <c r="G17" s="18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>344.25</v>
       </c>
       <c r="H17" s="18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>290.7</v>
       </c>
       <c r="I17" s="18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>290.7</v>
       </c>
       <c r="J17" s="11">
         <f>$B$17*(100-J11)/100</f>
         <v>260.10000000000002</v>
       </c>
-      <c r="K17" s="11"/>
+      <c r="K17" s="11">
+        <f>$B$17*(100-K11)/100</f>
+        <v>191.30312499999988</v>
+      </c>
       <c r="L17" s="11"/>
-      <c r="M17" s="20"/>
-      <c r="N17" s="18"/>
-    </row>
-    <row r="18" spans="1:14">
+      <c r="M17" s="11"/>
+      <c r="N17" s="20"/>
+      <c r="O17" s="18"/>
+    </row>
+    <row r="18" spans="1:15">
       <c r="A18" s="1" t="s">
         <v>4</v>
       </c>
@@ -1474,44 +1518,48 @@
       <c r="J18" s="11">
         <v>425</v>
       </c>
-      <c r="K18" s="11"/>
+      <c r="K18" s="11">
+        <v>585</v>
+      </c>
       <c r="L18" s="11"/>
-      <c r="M18" s="20"/>
-      <c r="N18" s="18"/>
-    </row>
-    <row r="21" spans="1:14">
+      <c r="M18" s="11"/>
+      <c r="N18" s="20"/>
+      <c r="O18" s="18"/>
+    </row>
+    <row r="21" spans="1:15">
       <c r="A21" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="4"/>
       <c r="D22" s="3"/>
     </row>
-    <row r="23" spans="1:14" ht="27.75" customHeight="1">
+    <row r="23" spans="1:15" ht="27.75" customHeight="1">
       <c r="A23" s="8"/>
-      <c r="B23" s="35"/>
-      <c r="C23" s="35"/>
-      <c r="D23" s="35"/>
-      <c r="E23" s="35"/>
-      <c r="F23" s="35"/>
-      <c r="G23" s="27"/>
+      <c r="B23" s="34"/>
+      <c r="C23" s="34"/>
+      <c r="D23" s="34"/>
+      <c r="E23" s="34"/>
+      <c r="F23" s="34"/>
+      <c r="G23" s="26"/>
       <c r="H23" s="8"/>
       <c r="I23" s="8"/>
       <c r="J23" s="8"/>
       <c r="K23" s="8"/>
       <c r="L23" s="8"/>
-      <c r="M23" s="9"/>
+      <c r="M23" s="8"/>
+      <c r="N23" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="D23:F23"/>
     <mergeCell ref="B23:C23"/>
-    <mergeCell ref="J5:M5"/>
+    <mergeCell ref="J5:N5"/>
   </mergeCells>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
 </worksheet>
@@ -1519,74 +1567,74 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L20"/>
+  <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K20" sqref="B5:K20"/>
+      <selection activeCell="K26" sqref="B3:K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="3" style="28" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3" style="27" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="3" style="28" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3" style="27" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="2.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="3" style="28" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="3" style="27" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="2.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="3" style="28" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="3" style="27" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="2.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="3" style="28" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="3" style="27" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="2.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="35" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36" t="s">
+      <c r="C1" s="35"/>
+      <c r="D1" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36" t="s">
+      <c r="E1" s="35"/>
+      <c r="F1" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36" t="s">
+      <c r="G1" s="35"/>
+      <c r="H1" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36" t="s">
+      <c r="I1" s="35"/>
+      <c r="J1" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="K1" s="36"/>
+      <c r="K1" s="35"/>
     </row>
     <row r="2" spans="1:12">
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="27" t="s">
         <v>42</v>
       </c>
       <c r="C2" t="s">
         <v>43</v>
       </c>
-      <c r="D2" s="28" t="s">
+      <c r="D2" s="27" t="s">
         <v>42</v>
       </c>
       <c r="E2" t="s">
         <v>43</v>
       </c>
-      <c r="F2" s="28" t="s">
+      <c r="F2" s="27" t="s">
         <v>42</v>
       </c>
       <c r="G2" t="s">
         <v>43</v>
       </c>
-      <c r="H2" s="28" t="s">
+      <c r="H2" s="27" t="s">
         <v>42</v>
       </c>
       <c r="I2" t="s">
         <v>43</v>
       </c>
-      <c r="J2" s="28" t="s">
+      <c r="J2" s="27" t="s">
         <v>42</v>
       </c>
       <c r="K2" t="s">
@@ -1607,16 +1655,16 @@
       <c r="A5" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="28">
+      <c r="B5" s="27">
         <v>3</v>
       </c>
-      <c r="F5" s="28">
+      <c r="F5" s="27">
         <v>3</v>
       </c>
-      <c r="H5" s="28">
+      <c r="H5" s="27">
         <v>2</v>
       </c>
-      <c r="J5" s="28">
+      <c r="J5" s="27">
         <v>3</v>
       </c>
       <c r="K5">
@@ -1627,22 +1675,22 @@
       <c r="A6" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="28">
+      <c r="B6" s="27">
         <v>4</v>
       </c>
-      <c r="D6" s="28">
+      <c r="D6" s="27">
         <v>4</v>
       </c>
-      <c r="F6" s="28">
+      <c r="F6" s="27">
         <v>4</v>
       </c>
       <c r="G6">
         <v>3</v>
       </c>
-      <c r="H6" s="28">
+      <c r="H6" s="27">
         <v>4</v>
       </c>
-      <c r="J6" s="28">
+      <c r="J6" s="27">
         <v>4</v>
       </c>
       <c r="K6">
@@ -1653,25 +1701,25 @@
       <c r="A7" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="28">
+      <c r="B7" s="27">
         <v>4</v>
       </c>
-      <c r="D7" s="28">
+      <c r="D7" s="27">
         <v>4</v>
       </c>
       <c r="E7">
         <v>4</v>
       </c>
-      <c r="F7" s="28">
+      <c r="F7" s="27">
         <v>4</v>
       </c>
       <c r="G7">
         <v>7</v>
       </c>
-      <c r="H7" s="28">
+      <c r="H7" s="27">
         <v>4</v>
       </c>
-      <c r="J7" s="28">
+      <c r="J7" s="27">
         <v>4</v>
       </c>
       <c r="K7">
@@ -1682,28 +1730,28 @@
       <c r="A8" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="28">
+      <c r="B8" s="27">
         <v>2.5</v>
       </c>
       <c r="C8">
         <v>4</v>
       </c>
-      <c r="D8" s="28">
+      <c r="D8" s="27">
         <v>2.5</v>
       </c>
-      <c r="F8" s="28">
+      <c r="F8" s="27">
         <v>2.5</v>
       </c>
       <c r="G8">
         <v>1</v>
       </c>
-      <c r="H8" s="28">
+      <c r="H8" s="27">
         <v>2.5</v>
       </c>
       <c r="I8">
         <v>4</v>
       </c>
-      <c r="J8" s="28">
+      <c r="J8" s="27">
         <v>2.5</v>
       </c>
       <c r="K8">
@@ -1714,22 +1762,22 @@
       <c r="A9" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="28">
+      <c r="B9" s="27">
         <v>2.5</v>
       </c>
       <c r="E9">
         <v>6</v>
       </c>
-      <c r="F9" s="28">
+      <c r="F9" s="27">
         <v>2.5</v>
       </c>
       <c r="G9">
         <v>9</v>
       </c>
-      <c r="H9" s="28">
+      <c r="H9" s="27">
         <v>2.5</v>
       </c>
-      <c r="J9" s="28">
+      <c r="J9" s="27">
         <v>3</v>
       </c>
       <c r="K9">
@@ -1740,25 +1788,25 @@
       <c r="A10" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="28">
+      <c r="B10" s="27">
         <v>4</v>
       </c>
       <c r="C10">
         <v>5</v>
       </c>
-      <c r="D10" s="28">
+      <c r="D10" s="27">
         <v>4</v>
       </c>
       <c r="E10" s="22">
         <v>6</v>
       </c>
-      <c r="F10" s="28">
+      <c r="F10" s="27">
         <v>4</v>
       </c>
       <c r="G10" s="22">
         <v>5</v>
       </c>
-      <c r="H10" s="28">
+      <c r="H10" s="27">
         <v>4</v>
       </c>
       <c r="I10">
@@ -1772,22 +1820,22 @@
       <c r="A11" t="s">
         <v>32</v>
       </c>
-      <c r="B11" s="28">
+      <c r="B11" s="27">
         <v>4</v>
       </c>
-      <c r="D11" s="28">
+      <c r="D11" s="27">
         <v>4</v>
       </c>
-      <c r="F11" s="28">
+      <c r="F11" s="27">
         <v>4</v>
       </c>
-      <c r="H11" s="28">
+      <c r="H11" s="27">
         <v>4</v>
       </c>
       <c r="I11" s="22">
         <v>2</v>
       </c>
-      <c r="J11" s="28">
+      <c r="J11" s="27">
         <v>4</v>
       </c>
       <c r="K11" s="22">
@@ -1798,22 +1846,22 @@
       <c r="A12" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="28">
+      <c r="B12" s="27">
         <v>4</v>
       </c>
-      <c r="D12" s="28">
+      <c r="D12" s="27">
         <v>4</v>
       </c>
-      <c r="F12" s="28">
+      <c r="F12" s="27">
         <v>4</v>
       </c>
       <c r="G12">
         <v>4</v>
       </c>
-      <c r="H12" s="28">
+      <c r="H12" s="27">
         <v>4</v>
       </c>
-      <c r="J12" s="28">
+      <c r="J12" s="27">
         <v>4</v>
       </c>
       <c r="K12" s="22">
@@ -1824,16 +1872,16 @@
       <c r="A13" t="s">
         <v>34</v>
       </c>
-      <c r="D13" s="28">
+      <c r="D13" s="27">
         <v>4</v>
       </c>
-      <c r="F13" s="28">
+      <c r="F13" s="27">
         <v>4</v>
       </c>
-      <c r="H13" s="28">
+      <c r="H13" s="27">
         <v>4</v>
       </c>
-      <c r="J13" s="28">
+      <c r="J13" s="27">
         <v>4</v>
       </c>
       <c r="K13" s="22">
@@ -1844,19 +1892,19 @@
       <c r="A14" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="28">
+      <c r="D14" s="27">
         <v>2</v>
       </c>
       <c r="E14">
         <v>2</v>
       </c>
-      <c r="F14" s="28">
+      <c r="F14" s="27">
         <v>2</v>
       </c>
-      <c r="H14" s="28">
+      <c r="H14" s="27">
         <v>2</v>
       </c>
-      <c r="J14" s="28">
+      <c r="J14" s="27">
         <v>2</v>
       </c>
       <c r="K14" s="22">
@@ -1867,16 +1915,16 @@
       <c r="A15" t="s">
         <v>45</v>
       </c>
-      <c r="D15" s="28">
+      <c r="D15" s="27">
         <v>8</v>
       </c>
-      <c r="F15" s="28">
+      <c r="F15" s="27">
         <v>7</v>
       </c>
-      <c r="H15" s="28">
+      <c r="H15" s="27">
         <v>8</v>
       </c>
-      <c r="J15" s="28">
+      <c r="J15" s="27">
         <v>8</v>
       </c>
       <c r="L15" t="s">
@@ -1887,16 +1935,16 @@
       <c r="A16" t="s">
         <v>36</v>
       </c>
-      <c r="B16" s="28">
+      <c r="B16" s="27">
         <v>4</v>
       </c>
-      <c r="D16" s="28">
+      <c r="D16" s="27">
         <v>4</v>
       </c>
-      <c r="F16" s="28">
+      <c r="F16" s="27">
         <v>3</v>
       </c>
-      <c r="H16" s="28">
+      <c r="H16" s="27">
         <v>4</v>
       </c>
       <c r="K16">
@@ -1904,22 +1952,22 @@
       </c>
     </row>
     <row r="17" spans="1:11">
-      <c r="A17" s="30">
+      <c r="A17" s="29">
         <v>40682</v>
       </c>
-      <c r="B17" s="28">
+      <c r="B17" s="27">
         <v>9</v>
       </c>
-      <c r="D17" s="28">
+      <c r="D17" s="27">
         <v>6</v>
       </c>
       <c r="G17">
         <v>3</v>
       </c>
-      <c r="H17" s="28">
+      <c r="H17" s="27">
         <v>9</v>
       </c>
-      <c r="J17" s="28">
+      <c r="J17" s="27">
         <v>9</v>
       </c>
       <c r="K17">
@@ -1928,35 +1976,35 @@
     </row>
     <row r="18" spans="1:11">
       <c r="A18" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="K18">
         <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:11">
-      <c r="A19" s="30">
+      <c r="A19" s="29">
         <v>40693</v>
       </c>
-      <c r="B19" s="28">
+      <c r="B19" s="27">
         <v>8</v>
       </c>
       <c r="C19">
         <v>13</v>
       </c>
-      <c r="D19" s="28">
+      <c r="D19" s="27">
         <v>8</v>
       </c>
-      <c r="F19" s="28">
+      <c r="F19" s="27">
         <v>8</v>
       </c>
-      <c r="H19" s="28">
+      <c r="H19" s="27">
         <v>8</v>
       </c>
       <c r="I19">
         <v>9</v>
       </c>
-      <c r="J19" s="28">
+      <c r="J19" s="27">
         <v>8</v>
       </c>
       <c r="K19">
@@ -1965,9 +2013,120 @@
     </row>
     <row r="20" spans="1:11">
       <c r="A20" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="K20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
+      <c r="A21" s="29">
+        <v>40700</v>
+      </c>
+      <c r="B21" s="27">
+        <v>7</v>
+      </c>
+      <c r="D21" s="27">
+        <v>7</v>
+      </c>
+      <c r="F21" s="27">
+        <v>7</v>
+      </c>
+      <c r="H21" s="27">
+        <v>7</v>
+      </c>
+      <c r="J21" s="27">
+        <v>7</v>
+      </c>
+      <c r="K21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
+      <c r="A22" s="29">
+        <v>40701</v>
+      </c>
+      <c r="B22" s="27">
+        <v>7</v>
+      </c>
+      <c r="D22" s="27">
+        <v>7</v>
+      </c>
+      <c r="F22" s="27">
+        <v>7</v>
+      </c>
+      <c r="H22" s="27">
+        <v>7</v>
+      </c>
+      <c r="J22" s="27">
+        <v>7</v>
+      </c>
+      <c r="K22" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11">
+      <c r="A23" s="29">
+        <v>40702</v>
+      </c>
+      <c r="B23" s="27">
+        <v>7</v>
+      </c>
+      <c r="D23" s="27">
+        <v>6</v>
+      </c>
+      <c r="F23" s="27">
+        <v>7</v>
+      </c>
+      <c r="J23" s="27">
+        <v>7</v>
+      </c>
+      <c r="K23" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11">
+      <c r="A24" s="29">
+        <v>40703</v>
+      </c>
+      <c r="B24" s="27">
+        <v>7</v>
+      </c>
+      <c r="D24" s="27">
+        <v>7</v>
+      </c>
+      <c r="F24" s="27">
+        <v>7</v>
+      </c>
+      <c r="J24" s="27">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11">
+      <c r="A25" s="29">
+        <v>40704</v>
+      </c>
+      <c r="B25" s="27">
+        <v>6</v>
+      </c>
+      <c r="D25" s="27">
+        <v>7</v>
+      </c>
+      <c r="F25" s="27">
+        <v>7</v>
+      </c>
+      <c r="J25" s="27">
+        <v>7</v>
+      </c>
+      <c r="K25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11">
+      <c r="A26" s="29">
+        <v>40707</v>
+      </c>
+      <c r="K26">
         <v>2</v>
       </c>
     </row>
@@ -1979,7 +2138,7 @@
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="B1:C1"/>
   </mergeCells>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1989,311 +2148,311 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="C1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D1" t="s">
         <v>91</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>92</v>
       </c>
-      <c r="E1" t="s">
-        <v>93</v>
-      </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="33" t="s">
+        <v>85</v>
+      </c>
+      <c r="C2" s="31">
+        <v>1</v>
+      </c>
+      <c r="D2" s="31">
+        <f>D4*$C$4+D9*$C$9</f>
+        <v>0.6635416666666667</v>
+      </c>
+      <c r="E2" s="31">
+        <f>E4*$C$4+E9*$C$9</f>
+        <v>0.66874999999999996</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="33"/>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="33" t="s">
         <v>86</v>
       </c>
-      <c r="C2" s="32">
-        <v>1</v>
-      </c>
-      <c r="D2" s="32">
-        <f>D4*$C$4+D9*$C$9</f>
-        <v>0.53541666666666665</v>
-      </c>
-      <c r="E2" s="32">
-        <f>E4*$C$4+E9*$C$9</f>
-        <v>0.56875000000000009</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="34"/>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="34" t="s">
-        <v>87</v>
-      </c>
-      <c r="C4" s="32">
+      <c r="C4" s="31">
         <v>0.25</v>
       </c>
-      <c r="D4" s="32">
-        <v>1</v>
-      </c>
-      <c r="E4" s="32">
+      <c r="D4" s="31">
+        <v>1</v>
+      </c>
+      <c r="E4" s="31">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="B5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="B6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="B7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="34" t="s">
-        <v>94</v>
-      </c>
-      <c r="C9" s="32">
+      <c r="A9" s="33" t="s">
+        <v>93</v>
+      </c>
+      <c r="C9" s="31">
         <v>0.75</v>
       </c>
-      <c r="D9" s="32">
+      <c r="D9" s="31">
         <f>D10*$C$10+D28*$C$28</f>
-        <v>0.38055555555555554</v>
-      </c>
-      <c r="E9" s="32">
+        <v>0.55138888888888893</v>
+      </c>
+      <c r="E9" s="31">
         <f>E10*$C$10+E28*$C$28</f>
-        <v>0.42500000000000004</v>
+        <v>0.55833333333333335</v>
       </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="34" t="s">
+      <c r="A10" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="C10" s="32">
-        <v>0.5</v>
-      </c>
-      <c r="D10" s="32">
+      <c r="C10" s="31">
+        <v>0.5</v>
+      </c>
+      <c r="D10" s="31">
         <f>D11*$C$11+D15*$C$15+D23*$C$23</f>
-        <v>0.46111111111111108</v>
-      </c>
-      <c r="E10" s="32">
+        <v>0.60277777777777775</v>
+      </c>
+      <c r="E10" s="31">
         <f>E11*$C$11+E15*$C$15+E23*$C$23</f>
-        <v>0.65</v>
+        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="34" t="s">
+      <c r="A11" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="C11" s="32">
+      <c r="C11" s="31">
         <f>1/3</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="D11" s="32">
+      <c r="D11" s="31">
         <f>AVERAGE(D12:D13)</f>
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="E11" s="32">
+        <v>0.6</v>
+      </c>
+      <c r="E11" s="31">
         <f>AVERAGE(E12:E13)</f>
         <v>0.5</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="B12" t="s">
-        <v>76</v>
-      </c>
-      <c r="D12" s="32">
+        <v>75</v>
+      </c>
+      <c r="D12" s="31">
         <v>0.6</v>
       </c>
-      <c r="E12" s="32">
+      <c r="E12" s="31">
         <v>0.6</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="B13" t="s">
-        <v>97</v>
-      </c>
-      <c r="D13" s="32">
-        <v>0.5</v>
-      </c>
-      <c r="E13" s="32">
+        <v>96</v>
+      </c>
+      <c r="D13" s="31">
+        <v>0.6</v>
+      </c>
+      <c r="E13" s="31">
         <v>0.4</v>
       </c>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="34" t="s">
+      <c r="A15" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="C15" s="32">
+      <c r="C15" s="31">
         <f>1/3</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="D15" s="32">
+      <c r="D15" s="31">
         <f>AVERAGE(D16:D21)</f>
-        <v>0.5</v>
-      </c>
-      <c r="E15" s="32">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="E15" s="31">
         <f>AVERAGE(E16:E21)</f>
-        <v>0.70000000000000007</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="B16" t="s">
-        <v>80</v>
-      </c>
-      <c r="D16" s="32">
-        <v>0.6</v>
-      </c>
-      <c r="E16" s="32">
-        <v>0.85</v>
+        <v>79</v>
+      </c>
+      <c r="D16" s="31">
+        <v>0.75</v>
+      </c>
+      <c r="E16" s="31">
+        <v>0.8</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="B17" t="s">
-        <v>77</v>
-      </c>
-      <c r="D17" s="32">
-        <v>0.5</v>
-      </c>
-      <c r="E17" s="32">
+        <v>76</v>
+      </c>
+      <c r="D17" s="31">
+        <v>0.75</v>
+      </c>
+      <c r="E17" s="31">
         <v>0.8</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="B18" t="s">
-        <v>78</v>
-      </c>
-      <c r="D18" s="32">
-        <v>0.5</v>
-      </c>
-      <c r="E18" s="32">
+        <v>77</v>
+      </c>
+      <c r="D18" s="31">
+        <v>0.75</v>
+      </c>
+      <c r="E18" s="31">
         <v>0.8</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="B19" t="s">
-        <v>79</v>
-      </c>
-      <c r="D19" s="32">
-        <v>0.5</v>
-      </c>
-      <c r="E19" s="32">
+        <v>78</v>
+      </c>
+      <c r="D19" s="31">
         <v>0.75</v>
+      </c>
+      <c r="E19" s="31">
+        <v>0.8</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="B20" t="s">
-        <v>95</v>
-      </c>
-      <c r="D20" s="32">
-        <v>0.5</v>
-      </c>
-      <c r="E20" s="32">
-        <v>0.6</v>
+        <v>94</v>
+      </c>
+      <c r="D20" s="31">
+        <v>0.75</v>
+      </c>
+      <c r="E20" s="31">
+        <v>0.8</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="B21" t="s">
-        <v>96</v>
-      </c>
-      <c r="D21" s="32">
-        <v>0.4</v>
-      </c>
-      <c r="E21" s="32">
-        <v>0.4</v>
+        <v>95</v>
+      </c>
+      <c r="D21" s="31">
+        <v>0.5</v>
+      </c>
+      <c r="E21" s="31">
+        <v>0.5</v>
       </c>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23" s="34" t="s">
+      <c r="A23" s="33" t="s">
         <v>65</v>
       </c>
-      <c r="C23" s="32">
+      <c r="C23" s="31">
         <f>1/3</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="D23" s="32">
+      <c r="D23" s="31">
         <f>AVERAGE(D24:D26)</f>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="E23" s="32">
+        <v>0.5</v>
+      </c>
+      <c r="E23" s="31">
         <f>AVERAGE(E24:E26)</f>
         <v>0.75</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="B24" t="s">
-        <v>81</v>
-      </c>
-      <c r="D24" s="32">
-        <v>0.5</v>
-      </c>
-      <c r="E24" s="32">
+        <v>80</v>
+      </c>
+      <c r="D24" s="31">
+        <v>0.5</v>
+      </c>
+      <c r="E24" s="31">
         <v>0.75</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="B25" t="s">
-        <v>82</v>
-      </c>
-      <c r="D25" s="32">
-        <v>0.25</v>
-      </c>
-      <c r="E25" s="32">
+        <v>81</v>
+      </c>
+      <c r="D25" s="31">
+        <v>0.5</v>
+      </c>
+      <c r="E25" s="31">
         <v>0.7</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="B26" t="s">
-        <v>83</v>
-      </c>
-      <c r="D26" s="32">
-        <v>0.25</v>
-      </c>
-      <c r="E26" s="32">
+        <v>82</v>
+      </c>
+      <c r="D26" s="31">
+        <v>0.5</v>
+      </c>
+      <c r="E26" s="31">
         <v>0.8</v>
       </c>
     </row>
     <row r="28" spans="1:5">
-      <c r="A28" s="34" t="s">
+      <c r="A28" s="33" t="s">
         <v>68</v>
       </c>
-      <c r="C28" s="32">
-        <v>0.5</v>
-      </c>
-      <c r="D28" s="32">
+      <c r="C28" s="31">
+        <v>0.5</v>
+      </c>
+      <c r="D28" s="31">
         <f>AVERAGE(D29:D30)</f>
-        <v>0.3</v>
-      </c>
-      <c r="E28" s="32">
+        <v>0.5</v>
+      </c>
+      <c r="E28" s="31">
         <f>AVERAGE(E29:E30)</f>
-        <v>0.2</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="B29" t="s">
-        <v>85</v>
-      </c>
-      <c r="D29" s="32">
-        <v>0.3</v>
-      </c>
-      <c r="E29" s="32">
-        <v>0.2</v>
+        <v>84</v>
+      </c>
+      <c r="D29" s="31">
+        <v>0.5</v>
+      </c>
+      <c r="E29" s="31">
+        <v>0.4</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="B30" t="s">
-        <v>84</v>
-      </c>
-      <c r="D30" s="32">
-        <v>0.3</v>
-      </c>
-      <c r="E30" s="32">
-        <v>0.2</v>
+        <v>83</v>
+      </c>
+      <c r="D30" s="31">
+        <v>0.5</v>
+      </c>
+      <c r="E30" s="31">
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>
@@ -2307,7 +2466,7 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C15"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2331,7 +2490,7 @@
         <f>$B$1*$C$1</f>
         <v>32.5</v>
       </c>
-      <c r="D2" s="30">
+      <c r="D2" s="29">
         <v>40576</v>
       </c>
     </row>
@@ -2343,7 +2502,7 @@
         <f t="shared" ref="B3:B14" si="0">$B$1*$C$1</f>
         <v>32.5</v>
       </c>
-      <c r="D3" s="30"/>
+      <c r="D3" s="29"/>
     </row>
     <row r="4" spans="1:5">
       <c r="A4">
@@ -2353,7 +2512,7 @@
         <f t="shared" si="0"/>
         <v>32.5</v>
       </c>
-      <c r="D4" s="30"/>
+      <c r="D4" s="29"/>
     </row>
     <row r="5" spans="1:5">
       <c r="A5">
@@ -2363,7 +2522,7 @@
         <f t="shared" si="0"/>
         <v>32.5</v>
       </c>
-      <c r="D5" s="30">
+      <c r="D5" s="29">
         <v>40597</v>
       </c>
     </row>
@@ -2375,7 +2534,7 @@
         <f t="shared" si="0"/>
         <v>32.5</v>
       </c>
-      <c r="D6" s="30"/>
+      <c r="D6" s="29"/>
     </row>
     <row r="7" spans="1:5">
       <c r="A7">
@@ -2385,7 +2544,7 @@
         <f t="shared" si="0"/>
         <v>32.5</v>
       </c>
-      <c r="D7" s="30"/>
+      <c r="D7" s="29"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8">
@@ -2395,7 +2554,7 @@
         <f t="shared" si="0"/>
         <v>32.5</v>
       </c>
-      <c r="D8" s="30"/>
+      <c r="D8" s="29"/>
     </row>
     <row r="9" spans="1:5">
       <c r="A9">
@@ -2405,7 +2564,7 @@
         <f t="shared" si="0"/>
         <v>32.5</v>
       </c>
-      <c r="D9" s="30"/>
+      <c r="D9" s="29"/>
     </row>
     <row r="10" spans="1:5">
       <c r="A10">
@@ -2415,7 +2574,7 @@
         <f t="shared" si="0"/>
         <v>32.5</v>
       </c>
-      <c r="D10" s="30">
+      <c r="D10" s="29">
         <v>40632</v>
       </c>
     </row>
@@ -2427,7 +2586,7 @@
         <f t="shared" si="0"/>
         <v>32.5</v>
       </c>
-      <c r="D11" s="30"/>
+      <c r="D11" s="29"/>
     </row>
     <row r="12" spans="1:5">
       <c r="A12">
@@ -2437,10 +2596,10 @@
         <f t="shared" si="0"/>
         <v>32.5</v>
       </c>
-      <c r="D12" s="30">
+      <c r="D12" s="29">
         <v>40653</v>
       </c>
-      <c r="E12" s="30">
+      <c r="E12" s="29">
         <v>40658</v>
       </c>
     </row>
@@ -2461,7 +2620,7 @@
         <f t="shared" si="0"/>
         <v>32.5</v>
       </c>
-      <c r="D14" s="30">
+      <c r="D14" s="29">
         <v>40667</v>
       </c>
     </row>
@@ -2470,7 +2629,7 @@
         <f>C1*5</f>
         <v>32.5</v>
       </c>
-      <c r="D15" s="30">
+      <c r="D15" s="29">
         <v>40693</v>
       </c>
     </row>
@@ -2482,7 +2641,7 @@
         <f>$B$1*$C$15</f>
         <v>162.5</v>
       </c>
-      <c r="D16" s="30">
+      <c r="D16" s="29">
         <v>40704</v>
       </c>
     </row>
@@ -2494,7 +2653,7 @@
         <f t="shared" ref="B17:B18" si="1">$B$1*$C$15</f>
         <v>162.5</v>
       </c>
-      <c r="D17" s="30">
+      <c r="D17" s="29">
         <v>40711</v>
       </c>
     </row>
@@ -2506,10 +2665,10 @@
         <f t="shared" si="1"/>
         <v>162.5</v>
       </c>
-      <c r="D18" s="30">
+      <c r="D18" s="29">
         <v>40715</v>
       </c>
-      <c r="E18" s="30">
+      <c r="E18" s="29">
         <v>40718</v>
       </c>
     </row>
@@ -2520,12 +2679,354 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="30">
+        <f>B2*D2+B26*D26</f>
+        <v>0.74993055555555566</v>
+      </c>
+      <c r="B1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G1" s="29">
+        <v>40699</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="B2" s="30">
+        <f>C3*E3+C16*E16+C22*E22</f>
+        <v>0.94986111111111127</v>
+      </c>
+      <c r="C2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" s="31">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="B3" s="30"/>
+      <c r="C3" s="31">
+        <f>D4*F4+D6*F6+D9*F9+D13*F13</f>
+        <v>0.95625000000000004</v>
+      </c>
+      <c r="D3" s="31" t="s">
+        <v>53</v>
+      </c>
+      <c r="E3">
+        <f>(100/3)%</f>
+        <v>0.33333333333333337</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="D4" s="31">
+        <f>E5*G5</f>
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>48</v>
+      </c>
+      <c r="F4" s="31">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="E5" s="31">
+        <v>1</v>
+      </c>
+      <c r="F5" t="s">
+        <v>49</v>
+      </c>
+      <c r="G5" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="D6" s="31">
+        <f>E7*G7+E8*G8</f>
+        <v>0.92500000000000004</v>
+      </c>
+      <c r="E6" t="s">
+        <v>50</v>
+      </c>
+      <c r="F6" s="31">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="E7" s="31">
+        <v>0.95</v>
+      </c>
+      <c r="F7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G7" s="31">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="E8" s="31">
+        <v>0.9</v>
+      </c>
+      <c r="F8" t="s">
+        <v>52</v>
+      </c>
+      <c r="G8" s="31">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="D9" s="31">
+        <f>E10*G10+E11*G11+E12*G12</f>
+        <v>0.92500000000000004</v>
+      </c>
+      <c r="E9" t="s">
+        <v>54</v>
+      </c>
+      <c r="F9" s="31">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="E10" s="31">
+        <v>1</v>
+      </c>
+      <c r="F10" t="s">
+        <v>55</v>
+      </c>
+      <c r="G10" s="31">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="E11" s="31">
+        <v>1</v>
+      </c>
+      <c r="F11" t="s">
+        <v>56</v>
+      </c>
+      <c r="G11" s="31">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="E12" s="31">
+        <v>0.85</v>
+      </c>
+      <c r="F12" t="s">
+        <v>57</v>
+      </c>
+      <c r="G12" s="31">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="D13" s="31">
+        <f>E14*G14+E15*G15</f>
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="E13" t="s">
+        <v>58</v>
+      </c>
+      <c r="F13" s="31">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="E14" s="31">
+        <v>1</v>
+      </c>
+      <c r="F14" t="s">
+        <v>48</v>
+      </c>
+      <c r="G14" s="31">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="E15" s="31">
+        <v>0.95</v>
+      </c>
+      <c r="F15" t="s">
+        <v>57</v>
+      </c>
+      <c r="G15" s="31">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="C16" s="31">
+        <f>D17*F17+D18*F18+D21*F21</f>
+        <v>0.96000000000000019</v>
+      </c>
+      <c r="D16" t="s">
+        <v>59</v>
+      </c>
+      <c r="E16">
+        <f>(100/3)%</f>
+        <v>0.33333333333333337</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7">
+      <c r="D17" s="31">
+        <v>1</v>
+      </c>
+      <c r="E17" t="s">
+        <v>60</v>
+      </c>
+      <c r="F17" s="31">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7">
+      <c r="D18" s="31">
+        <f>E19*G19+E20*G20</f>
+        <v>1</v>
+      </c>
+      <c r="E18" t="s">
+        <v>61</v>
+      </c>
+      <c r="F18" s="31">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7">
+      <c r="E19" s="31">
+        <v>1</v>
+      </c>
+      <c r="F19" t="s">
+        <v>62</v>
+      </c>
+      <c r="G19" s="31">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7">
+      <c r="E20" s="31">
+        <v>1</v>
+      </c>
+      <c r="F20" t="s">
+        <v>63</v>
+      </c>
+      <c r="G20" s="31">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7">
+      <c r="D21" s="31">
+        <v>0.9</v>
+      </c>
+      <c r="E21" t="s">
+        <v>64</v>
+      </c>
+      <c r="F21" s="31">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7">
+      <c r="C22">
+        <f>D23*F23+D24*F24+D25*F25</f>
+        <v>0.93333333333333346</v>
+      </c>
+      <c r="D22" t="s">
+        <v>65</v>
+      </c>
+      <c r="E22">
+        <f>(100/3)%</f>
+        <v>0.33333333333333337</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7">
+      <c r="D23" s="31">
+        <v>1</v>
+      </c>
+      <c r="E23" t="s">
+        <v>66</v>
+      </c>
+      <c r="F23">
+        <f>(100/3)%</f>
+        <v>0.33333333333333337</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7">
+      <c r="D24" s="31">
+        <v>1</v>
+      </c>
+      <c r="E24" t="s">
+        <v>67</v>
+      </c>
+      <c r="F24">
+        <f>(100/3)%</f>
+        <v>0.33333333333333337</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7">
+      <c r="D25" s="31">
+        <v>0.8</v>
+      </c>
+      <c r="E25" t="s">
+        <v>58</v>
+      </c>
+      <c r="F25">
+        <f>(100/3)%</f>
+        <v>0.33333333333333337</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7">
+      <c r="B26" s="31">
+        <f>C27*E27</f>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="C26" t="s">
+        <v>68</v>
+      </c>
+      <c r="D26" s="31">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7">
+      <c r="C27" s="31">
+        <f>D28*F28</f>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="D27" t="s">
+        <v>69</v>
+      </c>
+      <c r="E27" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7">
+      <c r="D28" s="31">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="E28" t="s">
+        <v>70</v>
+      </c>
+      <c r="F28" s="31">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G28"/>
   <sheetViews>
@@ -2536,36 +3037,36 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="31">
+      <c r="A1" s="30">
         <f>B2*D2+B26*D26</f>
         <v>0.65958333333333341</v>
       </c>
       <c r="B1" t="s">
         <v>71</v>
       </c>
-      <c r="G1" s="30">
+      <c r="G1" s="29">
         <v>40699</v>
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="B2" s="31">
+      <c r="B2" s="30">
         <f>C3*E3+C16*E16+C22*E22</f>
         <v>0.91916666666666691</v>
       </c>
       <c r="C2" t="s">
         <v>47</v>
       </c>
-      <c r="D2" s="32">
+      <c r="D2" s="31">
         <v>0.5</v>
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="B3" s="31"/>
-      <c r="C3" s="32">
+      <c r="B3" s="30"/>
+      <c r="C3" s="31">
         <f>D4*F4+D6*F6+D9*F9+D13*F13</f>
         <v>0.93750000000000011</v>
       </c>
-      <c r="D3" s="32" t="s">
+      <c r="D3" s="31" t="s">
         <v>53</v>
       </c>
       <c r="E3">
@@ -2574,143 +3075,143 @@
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="D4" s="32">
+      <c r="D4" s="31">
         <f>E5*G5</f>
         <v>1</v>
       </c>
       <c r="E4" t="s">
         <v>48</v>
       </c>
-      <c r="F4" s="32">
+      <c r="F4" s="31">
         <v>0.25</v>
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="E5" s="32">
+      <c r="E5" s="31">
         <v>1</v>
       </c>
       <c r="F5" t="s">
         <v>49</v>
       </c>
-      <c r="G5" s="32">
+      <c r="G5" s="31">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="D6" s="32">
+      <c r="D6" s="31">
         <f>E7*G7+E8*G8</f>
         <v>0.85000000000000009</v>
       </c>
       <c r="E6" t="s">
         <v>50</v>
       </c>
-      <c r="F6" s="32">
+      <c r="F6" s="31">
         <v>0.25</v>
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="E7" s="32">
+      <c r="E7" s="31">
         <v>0.9</v>
       </c>
       <c r="F7" t="s">
         <v>51</v>
       </c>
-      <c r="G7" s="32">
+      <c r="G7" s="31">
         <v>0.5</v>
       </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="E8" s="32">
+      <c r="E8" s="31">
         <v>0.8</v>
       </c>
       <c r="F8" t="s">
         <v>52</v>
       </c>
-      <c r="G8" s="32">
+      <c r="G8" s="31">
         <v>0.5</v>
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="D9" s="32">
+      <c r="D9" s="31">
         <f>E10*G10+E11*G11+E12*G12</f>
         <v>0.92500000000000004</v>
       </c>
       <c r="E9" t="s">
         <v>54</v>
       </c>
-      <c r="F9" s="32">
+      <c r="F9" s="31">
         <v>0.25</v>
       </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="E10" s="32">
+      <c r="E10" s="31">
         <v>1</v>
       </c>
       <c r="F10" t="s">
         <v>55</v>
       </c>
-      <c r="G10" s="32">
+      <c r="G10" s="31">
         <v>0.25</v>
       </c>
     </row>
     <row r="11" spans="1:7">
-      <c r="E11" s="32">
+      <c r="E11" s="31">
         <v>1</v>
       </c>
       <c r="F11" t="s">
         <v>56</v>
       </c>
-      <c r="G11" s="32">
+      <c r="G11" s="31">
         <v>0.25</v>
       </c>
     </row>
     <row r="12" spans="1:7">
-      <c r="E12" s="32">
+      <c r="E12" s="31">
         <v>0.85</v>
       </c>
       <c r="F12" t="s">
         <v>57</v>
       </c>
-      <c r="G12" s="32">
+      <c r="G12" s="31">
         <v>0.5</v>
       </c>
     </row>
     <row r="13" spans="1:7">
-      <c r="D13" s="32">
+      <c r="D13" s="31">
         <f>E14*G14+E15*G15</f>
         <v>0.97499999999999998</v>
       </c>
       <c r="E13" t="s">
         <v>58</v>
       </c>
-      <c r="F13" s="32">
+      <c r="F13" s="31">
         <v>0.25</v>
       </c>
     </row>
     <row r="14" spans="1:7">
-      <c r="E14" s="32">
+      <c r="E14" s="31">
         <v>1</v>
       </c>
       <c r="F14" t="s">
         <v>48</v>
       </c>
-      <c r="G14" s="32">
+      <c r="G14" s="31">
         <v>0.5</v>
       </c>
     </row>
     <row r="15" spans="1:7">
-      <c r="E15" s="32">
+      <c r="E15" s="31">
         <v>0.95</v>
       </c>
       <c r="F15" t="s">
         <v>57</v>
       </c>
-      <c r="G15" s="32">
+      <c r="G15" s="31">
         <v>0.5</v>
       </c>
     </row>
     <row r="16" spans="1:7">
-      <c r="C16" s="32">
+      <c r="C16" s="31">
         <f>D17*F17+D18*F18+D21*F21</f>
         <v>0.92000000000000015</v>
       </c>
@@ -2723,58 +3224,58 @@
       </c>
     </row>
     <row r="17" spans="2:7">
-      <c r="D17" s="32">
+      <c r="D17" s="31">
         <v>1</v>
       </c>
       <c r="E17" t="s">
         <v>60</v>
       </c>
-      <c r="F17" s="32">
+      <c r="F17" s="31">
         <v>0.2</v>
       </c>
     </row>
     <row r="18" spans="2:7">
-      <c r="D18" s="32">
+      <c r="D18" s="31">
         <f>E19*G19+E20*G20</f>
         <v>1</v>
       </c>
       <c r="E18" t="s">
         <v>61</v>
       </c>
-      <c r="F18" s="32">
+      <c r="F18" s="31">
         <v>0.4</v>
       </c>
     </row>
     <row r="19" spans="2:7">
-      <c r="E19" s="32">
+      <c r="E19" s="31">
         <v>1</v>
       </c>
       <c r="F19" t="s">
         <v>62</v>
       </c>
-      <c r="G19" s="32">
+      <c r="G19" s="31">
         <v>0.5</v>
       </c>
     </row>
     <row r="20" spans="2:7">
-      <c r="E20" s="32">
+      <c r="E20" s="31">
         <v>1</v>
       </c>
       <c r="F20" t="s">
         <v>63</v>
       </c>
-      <c r="G20" s="32">
+      <c r="G20" s="31">
         <v>0.5</v>
       </c>
     </row>
     <row r="21" spans="2:7">
-      <c r="D21" s="32">
+      <c r="D21" s="31">
         <v>0.8</v>
       </c>
       <c r="E21" t="s">
         <v>64</v>
       </c>
-      <c r="F21" s="32">
+      <c r="F21" s="31">
         <v>0.4</v>
       </c>
     </row>
@@ -2792,7 +3293,7 @@
       </c>
     </row>
     <row r="23" spans="2:7">
-      <c r="D23" s="32">
+      <c r="D23" s="31">
         <v>1</v>
       </c>
       <c r="E23" t="s">
@@ -2804,7 +3305,7 @@
       </c>
     </row>
     <row r="24" spans="2:7">
-      <c r="D24" s="32">
+      <c r="D24" s="31">
         <v>1</v>
       </c>
       <c r="E24" t="s">
@@ -2816,7 +3317,7 @@
       </c>
     </row>
     <row r="25" spans="2:7">
-      <c r="D25" s="32">
+      <c r="D25" s="31">
         <v>0.7</v>
       </c>
       <c r="E25" t="s">
@@ -2828,37 +3329,37 @@
       </c>
     </row>
     <row r="26" spans="2:7">
-      <c r="B26" s="32">
+      <c r="B26" s="31">
         <f>C27*E27</f>
         <v>0.4</v>
       </c>
       <c r="C26" t="s">
         <v>68</v>
       </c>
-      <c r="D26" s="32">
+      <c r="D26" s="31">
         <v>0.5</v>
       </c>
     </row>
     <row r="27" spans="2:7">
-      <c r="C27" s="32">
+      <c r="C27" s="31">
         <f>D28*F28</f>
         <v>0.4</v>
       </c>
       <c r="D27" t="s">
         <v>69</v>
       </c>
-      <c r="E27" s="32">
+      <c r="E27" s="31">
         <v>1</v>
       </c>
     </row>
     <row r="28" spans="2:7">
-      <c r="D28" s="32">
+      <c r="D28" s="31">
         <v>0.4</v>
       </c>
       <c r="E28" t="s">
         <v>70</v>
       </c>
-      <c r="F28" s="32">
+      <c r="F28" s="31">
         <v>1</v>
       </c>
     </row>
@@ -2867,7 +3368,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G28"/>
   <sheetViews>
@@ -2878,7 +3379,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="31">
+      <c r="A1" s="30">
         <f>B2*D2+B26*D26</f>
         <v>0.62798611111111113</v>
       </c>
@@ -2887,24 +3388,24 @@
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="B2" s="31">
+      <c r="B2" s="30">
         <f>C3*E3+C16*E16+C22*E22</f>
         <v>0.9059722222222224</v>
       </c>
       <c r="C2" t="s">
         <v>47</v>
       </c>
-      <c r="D2" s="32">
+      <c r="D2" s="31">
         <v>0.5</v>
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="B3" s="31"/>
-      <c r="C3" s="32">
+      <c r="B3" s="30"/>
+      <c r="C3" s="31">
         <f>D4*F4+D6*F6+D9*F9+D13*F13</f>
         <v>0.93125000000000002</v>
       </c>
-      <c r="D3" s="32" t="s">
+      <c r="D3" s="31" t="s">
         <v>53</v>
       </c>
       <c r="E3">
@@ -2913,143 +3414,143 @@
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="D4" s="32">
+      <c r="D4" s="31">
         <f>E5*G5</f>
         <v>1</v>
       </c>
       <c r="E4" t="s">
         <v>48</v>
       </c>
-      <c r="F4" s="32">
+      <c r="F4" s="31">
         <v>0.25</v>
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="E5" s="32">
+      <c r="E5" s="31">
         <v>1</v>
       </c>
       <c r="F5" t="s">
         <v>49</v>
       </c>
-      <c r="G5" s="32">
+      <c r="G5" s="31">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="D6" s="32">
+      <c r="D6" s="31">
         <f>E7*G7+E8*G8</f>
         <v>0.85000000000000009</v>
       </c>
       <c r="E6" t="s">
         <v>50</v>
       </c>
-      <c r="F6" s="32">
+      <c r="F6" s="31">
         <v>0.25</v>
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="E7" s="32">
+      <c r="E7" s="31">
         <v>0.9</v>
       </c>
       <c r="F7" t="s">
         <v>51</v>
       </c>
-      <c r="G7" s="32">
+      <c r="G7" s="31">
         <v>0.5</v>
       </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="E8" s="32">
+      <c r="E8" s="31">
         <v>0.8</v>
       </c>
       <c r="F8" t="s">
         <v>52</v>
       </c>
-      <c r="G8" s="32">
+      <c r="G8" s="31">
         <v>0.5</v>
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="D9" s="32">
+      <c r="D9" s="31">
         <f>E10*G10+E11*G11+E12*G12</f>
         <v>0.9</v>
       </c>
       <c r="E9" t="s">
         <v>54</v>
       </c>
-      <c r="F9" s="32">
+      <c r="F9" s="31">
         <v>0.25</v>
       </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="E10" s="32">
+      <c r="E10" s="31">
         <v>1</v>
       </c>
       <c r="F10" t="s">
         <v>55</v>
       </c>
-      <c r="G10" s="32">
+      <c r="G10" s="31">
         <v>0.25</v>
       </c>
     </row>
     <row r="11" spans="1:7">
-      <c r="E11" s="32">
+      <c r="E11" s="31">
         <v>1</v>
       </c>
       <c r="F11" t="s">
         <v>56</v>
       </c>
-      <c r="G11" s="32">
+      <c r="G11" s="31">
         <v>0.25</v>
       </c>
     </row>
     <row r="12" spans="1:7">
-      <c r="E12" s="32">
+      <c r="E12" s="31">
         <v>0.8</v>
       </c>
       <c r="F12" t="s">
         <v>57</v>
       </c>
-      <c r="G12" s="32">
+      <c r="G12" s="31">
         <v>0.5</v>
       </c>
     </row>
     <row r="13" spans="1:7">
-      <c r="D13" s="32">
+      <c r="D13" s="31">
         <f>E14*G14+E15*G15</f>
         <v>0.97499999999999998</v>
       </c>
       <c r="E13" t="s">
         <v>58</v>
       </c>
-      <c r="F13" s="32">
+      <c r="F13" s="31">
         <v>0.25</v>
       </c>
     </row>
     <row r="14" spans="1:7">
-      <c r="E14" s="32">
+      <c r="E14" s="31">
         <v>1</v>
       </c>
       <c r="F14" t="s">
         <v>48</v>
       </c>
-      <c r="G14" s="32">
+      <c r="G14" s="31">
         <v>0.5</v>
       </c>
     </row>
     <row r="15" spans="1:7">
-      <c r="E15" s="32">
+      <c r="E15" s="31">
         <v>0.95</v>
       </c>
       <c r="F15" t="s">
         <v>57</v>
       </c>
-      <c r="G15" s="32">
+      <c r="G15" s="31">
         <v>0.5</v>
       </c>
     </row>
     <row r="16" spans="1:7">
-      <c r="C16" s="32">
+      <c r="C16" s="31">
         <f>D17*F17+D18*F18+D21*F21</f>
         <v>0.92000000000000015</v>
       </c>
@@ -3062,58 +3563,58 @@
       </c>
     </row>
     <row r="17" spans="2:7">
-      <c r="D17" s="32">
+      <c r="D17" s="31">
         <v>1</v>
       </c>
       <c r="E17" t="s">
         <v>60</v>
       </c>
-      <c r="F17" s="32">
+      <c r="F17" s="31">
         <v>0.2</v>
       </c>
     </row>
     <row r="18" spans="2:7">
-      <c r="D18" s="32">
+      <c r="D18" s="31">
         <f>E19*G19+E20*G20</f>
         <v>1</v>
       </c>
       <c r="E18" t="s">
         <v>61</v>
       </c>
-      <c r="F18" s="32">
+      <c r="F18" s="31">
         <v>0.4</v>
       </c>
     </row>
     <row r="19" spans="2:7">
-      <c r="E19" s="32">
+      <c r="E19" s="31">
         <v>1</v>
       </c>
       <c r="F19" t="s">
         <v>62</v>
       </c>
-      <c r="G19" s="32">
+      <c r="G19" s="31">
         <v>0.5</v>
       </c>
     </row>
     <row r="20" spans="2:7">
-      <c r="E20" s="32">
+      <c r="E20" s="31">
         <v>1</v>
       </c>
       <c r="F20" t="s">
         <v>63</v>
       </c>
-      <c r="G20" s="32">
+      <c r="G20" s="31">
         <v>0.5</v>
       </c>
     </row>
     <row r="21" spans="2:7">
-      <c r="D21" s="32">
+      <c r="D21" s="31">
         <v>0.8</v>
       </c>
       <c r="E21" t="s">
         <v>64</v>
       </c>
-      <c r="F21" s="32">
+      <c r="F21" s="31">
         <v>0.4</v>
       </c>
     </row>
@@ -3131,7 +3632,7 @@
       </c>
     </row>
     <row r="23" spans="2:7">
-      <c r="D23" s="32">
+      <c r="D23" s="31">
         <v>1</v>
       </c>
       <c r="E23" t="s">
@@ -3143,7 +3644,7 @@
       </c>
     </row>
     <row r="24" spans="2:7">
-      <c r="D24" s="32">
+      <c r="D24" s="31">
         <v>1</v>
       </c>
       <c r="E24" t="s">
@@ -3155,7 +3656,7 @@
       </c>
     </row>
     <row r="25" spans="2:7">
-      <c r="D25" s="32">
+      <c r="D25" s="31">
         <v>0.6</v>
       </c>
       <c r="E25" t="s">
@@ -3167,376 +3668,37 @@
       </c>
     </row>
     <row r="26" spans="2:7">
-      <c r="B26" s="32">
+      <c r="B26" s="31">
         <f>C27*E27</f>
         <v>0.35</v>
       </c>
       <c r="C26" t="s">
         <v>68</v>
       </c>
-      <c r="D26" s="32">
+      <c r="D26" s="31">
         <v>0.5</v>
       </c>
     </row>
     <row r="27" spans="2:7">
-      <c r="C27" s="32">
+      <c r="C27" s="31">
         <f>D28*F28</f>
         <v>0.35</v>
       </c>
       <c r="D27" t="s">
         <v>69</v>
       </c>
-      <c r="E27" s="32">
+      <c r="E27" s="31">
         <v>1</v>
       </c>
     </row>
     <row r="28" spans="2:7">
-      <c r="D28" s="32">
+      <c r="D28" s="31">
         <v>0.35</v>
       </c>
       <c r="E28" t="s">
         <v>70</v>
       </c>
-      <c r="F28" s="32">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G28"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A48" sqref="A48"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" s="31">
-        <f>B2*D2+B26*D26</f>
-        <v>0.5573611111111112</v>
-      </c>
-      <c r="B1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="B2" s="31">
-        <f>C3*E3+C16*E16+C22*E22</f>
-        <v>0.91472222222222244</v>
-      </c>
-      <c r="C2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D2" s="32">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="B3" s="31"/>
-      <c r="C3" s="32">
-        <f>D4*F4+D6*F6+D9*F9+D13*F13</f>
-        <v>0.91250000000000009</v>
-      </c>
-      <c r="D3" s="32" t="s">
-        <v>53</v>
-      </c>
-      <c r="E3">
-        <f>(100/3)%</f>
-        <v>0.33333333333333337</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="D4" s="32">
-        <f>E5*G5</f>
-        <v>1</v>
-      </c>
-      <c r="E4" t="s">
-        <v>48</v>
-      </c>
-      <c r="F4" s="32">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="E5" s="32">
-        <v>1</v>
-      </c>
-      <c r="F5" t="s">
-        <v>49</v>
-      </c>
-      <c r="G5" s="32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="D6" s="32">
-        <f>E7*G7+E8*G8</f>
-        <v>0.85000000000000009</v>
-      </c>
-      <c r="E6" t="s">
-        <v>50</v>
-      </c>
-      <c r="F6" s="32">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="E7" s="32">
-        <v>0.9</v>
-      </c>
-      <c r="F7" t="s">
-        <v>51</v>
-      </c>
-      <c r="G7" s="32">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="E8" s="32">
-        <v>0.8</v>
-      </c>
-      <c r="F8" t="s">
-        <v>52</v>
-      </c>
-      <c r="G8" s="32">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="D9" s="32">
-        <f>E10*G10+E11*G11+E12*G12</f>
-        <v>0.85</v>
-      </c>
-      <c r="E9" t="s">
-        <v>54</v>
-      </c>
-      <c r="F9" s="32">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="E10" s="32">
-        <v>1</v>
-      </c>
-      <c r="F10" t="s">
-        <v>55</v>
-      </c>
-      <c r="G10" s="32">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="E11" s="32">
-        <v>1</v>
-      </c>
-      <c r="F11" t="s">
-        <v>56</v>
-      </c>
-      <c r="G11" s="32">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="E12" s="32">
-        <v>0.7</v>
-      </c>
-      <c r="F12" t="s">
-        <v>57</v>
-      </c>
-      <c r="G12" s="32">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="D13" s="32">
-        <f>E14*G14+E15*G15</f>
-        <v>0.95</v>
-      </c>
-      <c r="E13" t="s">
-        <v>58</v>
-      </c>
-      <c r="F13" s="32">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="E14" s="32">
-        <v>1</v>
-      </c>
-      <c r="F14" t="s">
-        <v>48</v>
-      </c>
-      <c r="G14" s="32">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="E15" s="32">
-        <v>0.9</v>
-      </c>
-      <c r="F15" t="s">
-        <v>57</v>
-      </c>
-      <c r="G15" s="32">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="C16" s="32">
-        <f>D17*F17+D18*F18+D21*F21</f>
-        <v>0.96500000000000008</v>
-      </c>
-      <c r="D16" t="s">
-        <v>59</v>
-      </c>
-      <c r="E16">
-        <f>(100/3)%</f>
-        <v>0.33333333333333337</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7">
-      <c r="D17" s="32">
-        <v>1</v>
-      </c>
-      <c r="E17" t="s">
-        <v>60</v>
-      </c>
-      <c r="F17" s="32">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7">
-      <c r="D18" s="32">
-        <f>E19*G19+E20*G20</f>
-        <v>1</v>
-      </c>
-      <c r="E18" t="s">
-        <v>61</v>
-      </c>
-      <c r="F18" s="32">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="19" spans="2:7">
-      <c r="E19" s="32">
-        <v>1</v>
-      </c>
-      <c r="F19" t="s">
-        <v>62</v>
-      </c>
-      <c r="G19" s="32">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="20" spans="2:7">
-      <c r="E20" s="32">
-        <v>1</v>
-      </c>
-      <c r="F20" t="s">
-        <v>63</v>
-      </c>
-      <c r="G20" s="32">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="21" spans="2:7">
-      <c r="D21" s="32">
-        <v>0.7</v>
-      </c>
-      <c r="E21" t="s">
-        <v>64</v>
-      </c>
-      <c r="F21" s="32">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="22" spans="2:7">
-      <c r="C22">
-        <f>D23*F23+D24*F24+D25*F25</f>
-        <v>0.8666666666666667</v>
-      </c>
-      <c r="D22" t="s">
-        <v>65</v>
-      </c>
-      <c r="E22">
-        <f>(100/3)%</f>
-        <v>0.33333333333333337</v>
-      </c>
-    </row>
-    <row r="23" spans="2:7">
-      <c r="D23" s="32">
-        <v>1</v>
-      </c>
-      <c r="E23" t="s">
-        <v>66</v>
-      </c>
-      <c r="F23">
-        <f>(100/3)%</f>
-        <v>0.33333333333333337</v>
-      </c>
-    </row>
-    <row r="24" spans="2:7">
-      <c r="D24" s="32">
-        <v>1</v>
-      </c>
-      <c r="E24" t="s">
-        <v>67</v>
-      </c>
-      <c r="F24">
-        <f>(100/3)%</f>
-        <v>0.33333333333333337</v>
-      </c>
-    </row>
-    <row r="25" spans="2:7">
-      <c r="D25" s="32">
-        <v>0.6</v>
-      </c>
-      <c r="E25" t="s">
-        <v>58</v>
-      </c>
-      <c r="F25">
-        <f>(100/3)%</f>
-        <v>0.33333333333333337</v>
-      </c>
-    </row>
-    <row r="26" spans="2:7">
-      <c r="B26" s="32">
-        <f>C27*E27</f>
-        <v>0.2</v>
-      </c>
-      <c r="C26" t="s">
-        <v>68</v>
-      </c>
-      <c r="D26" s="32">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="27" spans="2:7">
-      <c r="C27" s="32">
-        <f>D28*F28</f>
-        <v>0.2</v>
-      </c>
-      <c r="D27" t="s">
-        <v>69</v>
-      </c>
-      <c r="E27" s="32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="2:7">
-      <c r="D28" s="32">
-        <v>0.2</v>
-      </c>
-      <c r="E28" t="s">
-        <v>70</v>
-      </c>
-      <c r="F28" s="32">
+      <c r="F28" s="31">
         <v>1</v>
       </c>
     </row>
@@ -3556,36 +3718,36 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="31">
+      <c r="A1" s="30">
         <f>B2*D2+B26*D26</f>
         <v>0.31430555555555562</v>
       </c>
       <c r="B1" t="s">
         <v>71</v>
       </c>
-      <c r="D1" s="30">
+      <c r="D1" s="29">
         <v>40632</v>
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="B2" s="31">
+      <c r="B2" s="30">
         <f>C3*E3+C16*E16+C22*E22</f>
         <v>0.62861111111111123</v>
       </c>
       <c r="C2" t="s">
         <v>47</v>
       </c>
-      <c r="D2" s="32">
+      <c r="D2" s="31">
         <v>0.5</v>
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="B3" s="31"/>
-      <c r="C3" s="32">
+      <c r="B3" s="30"/>
+      <c r="C3" s="31">
         <f>D4*F4+D6*F6+D9*F9+D13*F13</f>
         <v>0.72500000000000009</v>
       </c>
-      <c r="D3" s="32" t="s">
+      <c r="D3" s="31" t="s">
         <v>53</v>
       </c>
       <c r="E3">
@@ -3594,142 +3756,142 @@
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="D4" s="32">
+      <c r="D4" s="31">
         <f>E5*G5</f>
         <v>1</v>
       </c>
       <c r="E4" t="s">
         <v>48</v>
       </c>
-      <c r="F4" s="32">
+      <c r="F4" s="31">
         <v>0.25</v>
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="E5" s="32">
+      <c r="E5" s="31">
         <v>1</v>
       </c>
       <c r="F5" t="s">
         <v>49</v>
       </c>
-      <c r="G5" s="32">
+      <c r="G5" s="31">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="D6" s="32">
+      <c r="D6" s="31">
         <f>E7*G7+E8*G8</f>
         <v>0.85000000000000009</v>
       </c>
       <c r="E6" t="s">
         <v>50</v>
       </c>
-      <c r="F6" s="32">
+      <c r="F6" s="31">
         <v>0.25</v>
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="E7" s="32">
+      <c r="E7" s="31">
         <v>0.9</v>
       </c>
       <c r="F7" t="s">
         <v>51</v>
       </c>
-      <c r="G7" s="32">
+      <c r="G7" s="31">
         <v>0.5</v>
       </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="E8" s="32">
+      <c r="E8" s="31">
         <v>0.8</v>
       </c>
       <c r="F8" t="s">
         <v>52</v>
       </c>
-      <c r="G8" s="32">
+      <c r="G8" s="31">
         <v>0.5</v>
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="D9" s="32">
+      <c r="D9" s="31">
         <f>E10*G10+E11*G11+E12*G12</f>
         <v>0.85</v>
       </c>
       <c r="E9" t="s">
         <v>54</v>
       </c>
-      <c r="F9" s="32">
+      <c r="F9" s="31">
         <v>0.25</v>
       </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="E10" s="32">
+      <c r="E10" s="31">
         <v>1</v>
       </c>
       <c r="F10" t="s">
         <v>55</v>
       </c>
-      <c r="G10" s="32">
+      <c r="G10" s="31">
         <v>0.25</v>
       </c>
     </row>
     <row r="11" spans="1:7">
-      <c r="E11" s="32">
+      <c r="E11" s="31">
         <v>1</v>
       </c>
       <c r="F11" t="s">
         <v>56</v>
       </c>
-      <c r="G11" s="32">
+      <c r="G11" s="31">
         <v>0.25</v>
       </c>
     </row>
     <row r="12" spans="1:7">
-      <c r="E12" s="32">
+      <c r="E12" s="31">
         <v>0.7</v>
       </c>
       <c r="F12" t="s">
         <v>57</v>
       </c>
-      <c r="G12" s="32">
+      <c r="G12" s="31">
         <v>0.5</v>
       </c>
     </row>
     <row r="13" spans="1:7">
-      <c r="D13" s="32">
+      <c r="D13" s="31">
         <v>0.2</v>
       </c>
       <c r="E13" t="s">
         <v>58</v>
       </c>
-      <c r="F13" s="32">
+      <c r="F13" s="31">
         <v>0.25</v>
       </c>
     </row>
     <row r="14" spans="1:7">
-      <c r="E14" s="32">
+      <c r="E14" s="31">
         <v>1</v>
       </c>
       <c r="F14" t="s">
         <v>48</v>
       </c>
-      <c r="G14" s="32">
+      <c r="G14" s="31">
         <v>0.5</v>
       </c>
     </row>
     <row r="15" spans="1:7">
-      <c r="E15" s="32">
+      <c r="E15" s="31">
         <v>0.9</v>
       </c>
       <c r="F15" t="s">
         <v>57</v>
       </c>
-      <c r="G15" s="32">
+      <c r="G15" s="31">
         <v>0.5</v>
       </c>
     </row>
     <row r="16" spans="1:7">
-      <c r="C16" s="32">
+      <c r="C16" s="31">
         <f>D17*F17+D18*F18+D21*F21</f>
         <v>0.62750000000000006</v>
       </c>
@@ -3742,57 +3904,57 @@
       </c>
     </row>
     <row r="17" spans="2:7">
-      <c r="D17" s="32">
+      <c r="D17" s="31">
         <v>1</v>
       </c>
       <c r="E17" t="s">
         <v>60</v>
       </c>
-      <c r="F17" s="32">
+      <c r="F17" s="31">
         <v>0.2</v>
       </c>
     </row>
     <row r="18" spans="2:7">
-      <c r="D18" s="32">
+      <c r="D18" s="31">
         <v>0.75</v>
       </c>
       <c r="E18" t="s">
         <v>61</v>
       </c>
-      <c r="F18" s="32">
+      <c r="F18" s="31">
         <v>0.45</v>
       </c>
     </row>
     <row r="19" spans="2:7">
-      <c r="E19" s="32">
+      <c r="E19" s="31">
         <v>1</v>
       </c>
       <c r="F19" t="s">
         <v>62</v>
       </c>
-      <c r="G19" s="32">
+      <c r="G19" s="31">
         <v>0.5</v>
       </c>
     </row>
     <row r="20" spans="2:7">
-      <c r="E20" s="32">
+      <c r="E20" s="31">
         <v>1</v>
       </c>
       <c r="F20" t="s">
         <v>63</v>
       </c>
-      <c r="G20" s="32">
+      <c r="G20" s="31">
         <v>0.5</v>
       </c>
     </row>
     <row r="21" spans="2:7">
-      <c r="D21" s="32">
+      <c r="D21" s="31">
         <v>0.2</v>
       </c>
       <c r="E21" t="s">
         <v>64</v>
       </c>
-      <c r="F21" s="32">
+      <c r="F21" s="31">
         <v>0.45</v>
       </c>
     </row>
@@ -3810,7 +3972,7 @@
       </c>
     </row>
     <row r="23" spans="2:7">
-      <c r="D23" s="32">
+      <c r="D23" s="31">
         <v>1</v>
       </c>
       <c r="E23" t="s">
@@ -3822,7 +3984,7 @@
       </c>
     </row>
     <row r="24" spans="2:7">
-      <c r="D24" s="32">
+      <c r="D24" s="31">
         <v>0.6</v>
       </c>
       <c r="E24" t="s">
@@ -3834,7 +3996,7 @@
       </c>
     </row>
     <row r="25" spans="2:7">
-      <c r="D25" s="32">
+      <c r="D25" s="31">
         <v>0</v>
       </c>
       <c r="E25" t="s">
@@ -3846,37 +4008,376 @@
       </c>
     </row>
     <row r="26" spans="2:7">
-      <c r="B26" s="32">
+      <c r="B26" s="31">
         <f>C27*E27</f>
         <v>0</v>
       </c>
       <c r="C26" t="s">
         <v>68</v>
       </c>
-      <c r="D26" s="32">
+      <c r="D26" s="31">
         <v>0.5</v>
       </c>
     </row>
     <row r="27" spans="2:7">
-      <c r="C27" s="32">
+      <c r="C27" s="31">
         <f>D28*F28</f>
         <v>0</v>
       </c>
       <c r="D27" t="s">
         <v>69</v>
       </c>
-      <c r="E27" s="32">
+      <c r="E27" s="31">
         <v>1</v>
       </c>
     </row>
     <row r="28" spans="2:7">
-      <c r="D28" s="32">
+      <c r="D28" s="31">
         <v>0</v>
       </c>
       <c r="E28" t="s">
         <v>70</v>
       </c>
-      <c r="F28" s="32">
+      <c r="F28" s="31">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A48" sqref="A48"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="30">
+        <f>B2*D2+B26*D26</f>
+        <v>0.5573611111111112</v>
+      </c>
+      <c r="B1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="B2" s="30">
+        <f>C3*E3+C16*E16+C22*E22</f>
+        <v>0.91472222222222244</v>
+      </c>
+      <c r="C2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" s="31">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="B3" s="30"/>
+      <c r="C3" s="31">
+        <f>D4*F4+D6*F6+D9*F9+D13*F13</f>
+        <v>0.91250000000000009</v>
+      </c>
+      <c r="D3" s="31" t="s">
+        <v>53</v>
+      </c>
+      <c r="E3">
+        <f>(100/3)%</f>
+        <v>0.33333333333333337</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="D4" s="31">
+        <f>E5*G5</f>
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>48</v>
+      </c>
+      <c r="F4" s="31">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="E5" s="31">
+        <v>1</v>
+      </c>
+      <c r="F5" t="s">
+        <v>49</v>
+      </c>
+      <c r="G5" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="D6" s="31">
+        <f>E7*G7+E8*G8</f>
+        <v>0.85000000000000009</v>
+      </c>
+      <c r="E6" t="s">
+        <v>50</v>
+      </c>
+      <c r="F6" s="31">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="E7" s="31">
+        <v>0.9</v>
+      </c>
+      <c r="F7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G7" s="31">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="E8" s="31">
+        <v>0.8</v>
+      </c>
+      <c r="F8" t="s">
+        <v>52</v>
+      </c>
+      <c r="G8" s="31">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="D9" s="31">
+        <f>E10*G10+E11*G11+E12*G12</f>
+        <v>0.85</v>
+      </c>
+      <c r="E9" t="s">
+        <v>54</v>
+      </c>
+      <c r="F9" s="31">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="E10" s="31">
+        <v>1</v>
+      </c>
+      <c r="F10" t="s">
+        <v>55</v>
+      </c>
+      <c r="G10" s="31">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="E11" s="31">
+        <v>1</v>
+      </c>
+      <c r="F11" t="s">
+        <v>56</v>
+      </c>
+      <c r="G11" s="31">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="E12" s="31">
+        <v>0.7</v>
+      </c>
+      <c r="F12" t="s">
+        <v>57</v>
+      </c>
+      <c r="G12" s="31">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="D13" s="31">
+        <f>E14*G14+E15*G15</f>
+        <v>0.95</v>
+      </c>
+      <c r="E13" t="s">
+        <v>58</v>
+      </c>
+      <c r="F13" s="31">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="E14" s="31">
+        <v>1</v>
+      </c>
+      <c r="F14" t="s">
+        <v>48</v>
+      </c>
+      <c r="G14" s="31">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="E15" s="31">
+        <v>0.9</v>
+      </c>
+      <c r="F15" t="s">
+        <v>57</v>
+      </c>
+      <c r="G15" s="31">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="C16" s="31">
+        <f>D17*F17+D18*F18+D21*F21</f>
+        <v>0.96500000000000008</v>
+      </c>
+      <c r="D16" t="s">
+        <v>59</v>
+      </c>
+      <c r="E16">
+        <f>(100/3)%</f>
+        <v>0.33333333333333337</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7">
+      <c r="D17" s="31">
+        <v>1</v>
+      </c>
+      <c r="E17" t="s">
+        <v>60</v>
+      </c>
+      <c r="F17" s="31">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7">
+      <c r="D18" s="31">
+        <f>E19*G19+E20*G20</f>
+        <v>1</v>
+      </c>
+      <c r="E18" t="s">
+        <v>61</v>
+      </c>
+      <c r="F18" s="31">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7">
+      <c r="E19" s="31">
+        <v>1</v>
+      </c>
+      <c r="F19" t="s">
+        <v>62</v>
+      </c>
+      <c r="G19" s="31">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7">
+      <c r="E20" s="31">
+        <v>1</v>
+      </c>
+      <c r="F20" t="s">
+        <v>63</v>
+      </c>
+      <c r="G20" s="31">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7">
+      <c r="D21" s="31">
+        <v>0.7</v>
+      </c>
+      <c r="E21" t="s">
+        <v>64</v>
+      </c>
+      <c r="F21" s="31">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7">
+      <c r="C22">
+        <f>D23*F23+D24*F24+D25*F25</f>
+        <v>0.8666666666666667</v>
+      </c>
+      <c r="D22" t="s">
+        <v>65</v>
+      </c>
+      <c r="E22">
+        <f>(100/3)%</f>
+        <v>0.33333333333333337</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7">
+      <c r="D23" s="31">
+        <v>1</v>
+      </c>
+      <c r="E23" t="s">
+        <v>66</v>
+      </c>
+      <c r="F23">
+        <f>(100/3)%</f>
+        <v>0.33333333333333337</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7">
+      <c r="D24" s="31">
+        <v>1</v>
+      </c>
+      <c r="E24" t="s">
+        <v>67</v>
+      </c>
+      <c r="F24">
+        <f>(100/3)%</f>
+        <v>0.33333333333333337</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7">
+      <c r="D25" s="31">
+        <v>0.6</v>
+      </c>
+      <c r="E25" t="s">
+        <v>58</v>
+      </c>
+      <c r="F25">
+        <f>(100/3)%</f>
+        <v>0.33333333333333337</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7">
+      <c r="B26" s="31">
+        <f>C27*E27</f>
+        <v>0.2</v>
+      </c>
+      <c r="C26" t="s">
+        <v>68</v>
+      </c>
+      <c r="D26" s="31">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7">
+      <c r="C27" s="31">
+        <f>D28*F28</f>
+        <v>0.2</v>
+      </c>
+      <c r="D27" t="s">
+        <v>69</v>
+      </c>
+      <c r="E27" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7">
+      <c r="D28" s="31">
+        <v>0.2</v>
+      </c>
+      <c r="E28" t="s">
+        <v>70</v>
+      </c>
+      <c r="F28" s="31">
         <v>1</v>
       </c>
     </row>

</xml_diff>